<commit_message>
Finish test for importing excel file
</commit_message>
<xml_diff>
--- a/HonglornAUT/TestData/ImportTemplate.xlsx
+++ b/HonglornAUT/TestData/ImportTemplate.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C695E17B-7B54-4424-847D-09F25075BCA5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ECC33CC-126F-4F87-95C7-BC9C802BABF8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Nachname</t>
   </si>
@@ -42,36 +42,6 @@
   </si>
   <si>
     <t>M</t>
-  </si>
-  <si>
-    <t>Bishop</t>
-  </si>
-  <si>
-    <t>John</t>
-  </si>
-  <si>
-    <t>Murray</t>
-  </si>
-  <si>
-    <t>Joyce</t>
-  </si>
-  <si>
-    <t>W</t>
-  </si>
-  <si>
-    <t>Griffin</t>
-  </si>
-  <si>
-    <t>Willie</t>
-  </si>
-  <si>
-    <t>05B</t>
-  </si>
-  <si>
-    <t>E03</t>
-  </si>
-  <si>
-    <t>5A</t>
   </si>
 </sst>
 </file>
@@ -396,10 +366,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -445,59 +415,8 @@
         <v>2005</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3">
-        <v>2005</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4">
-        <v>2004</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5">
-        <v>2005</v>
-      </c>
-    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F5">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F2">
     <sortCondition ref="F2"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>